<commit_message>
ignore log files and executables folder
</commit_message>
<xml_diff>
--- a/target/test-classes/excel/testData.xlsx
+++ b/target/test-classes/excel/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\eclipse_projects\Data-Driven-Framework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4202E21F-03A0-4316-ACAA-1AF86F7FE3B8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1CF257A-1BF4-4EAC-A3C5-90A3B0EF817D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="2160" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -378,14 +378,14 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>